<commit_message>
Adjust user authentication module
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I119"/>
+  <dimension ref="A1:I120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4850,6 +4850,43 @@
         <v>268</v>
       </c>
       <c r="I119" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>45906.43944444445</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>0x01,0x0C</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>380</v>
+      </c>
+      <c r="G120" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H120" t="n">
+        <v>268</v>
+      </c>
+      <c r="I120" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4864,7 +4901,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I119"/>
+  <dimension ref="A1:I120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9282,6 +9319,43 @@
         <v>276</v>
       </c>
       <c r="I119" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>45906.43944444445</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>0x01,0x10</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>380</v>
+      </c>
+      <c r="G120" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H120" t="n">
+        <v>272</v>
+      </c>
+      <c r="I120" t="n">
         <v>14</v>
       </c>
     </row>
@@ -9296,7 +9370,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I119"/>
+  <dimension ref="A1:I120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13714,6 +13788,43 @@
         <v>112</v>
       </c>
       <c r="I119" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>45906.43944444445</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>0x00,0x70</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>130</v>
+      </c>
+      <c r="G120" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H120" t="n">
+        <v>112</v>
+      </c>
+      <c r="I120" t="n">
         <v>7</v>
       </c>
     </row>
@@ -13728,7 +13839,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I119"/>
+  <dimension ref="A1:I120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18149,6 +18260,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>45906.43944444445</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>0x00,0x6F</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>130</v>
+      </c>
+      <c r="G120" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H120" t="n">
+        <v>111</v>
+      </c>
+      <c r="I120" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix database schema migration
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4924,6 +4924,43 @@
         <v>268</v>
       </c>
       <c r="I121" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>45908.43340277778</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>0x01,0x0C</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>380</v>
+      </c>
+      <c r="G122" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H122" t="n">
+        <v>268</v>
+      </c>
+      <c r="I122" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4938,7 +4975,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9430,6 +9467,43 @@
         <v>272</v>
       </c>
       <c r="I121" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>45908.43340277778</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>0x01,0x10</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>380</v>
+      </c>
+      <c r="G122" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H122" t="n">
+        <v>272</v>
+      </c>
+      <c r="I122" t="n">
         <v>14</v>
       </c>
     </row>
@@ -9444,7 +9518,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13936,6 +14010,43 @@
         <v>112</v>
       </c>
       <c r="I121" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>45908.43340277778</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>0x00,0x70</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>130</v>
+      </c>
+      <c r="G122" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H122" t="n">
+        <v>112</v>
+      </c>
+      <c r="I122" t="n">
         <v>7</v>
       </c>
     </row>
@@ -13950,7 +14061,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18445,6 +18556,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>45908.43340277778</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>0x00,0x6E</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>130</v>
+      </c>
+      <c r="G122" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H122" t="n">
+        <v>110</v>
+      </c>
+      <c r="I122" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revise responsive design implementation
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4961,6 +4961,43 @@
         <v>268</v>
       </c>
       <c r="I122" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>45909.4343287037</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>0x01,0x08</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>380</v>
+      </c>
+      <c r="G123" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H123" t="n">
+        <v>264</v>
+      </c>
+      <c r="I123" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4975,7 +5012,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9504,6 +9541,43 @@
         <v>272</v>
       </c>
       <c r="I122" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>45909.4343287037</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>0x01,0x10</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>380</v>
+      </c>
+      <c r="G123" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H123" t="n">
+        <v>272</v>
+      </c>
+      <c r="I123" t="n">
         <v>14</v>
       </c>
     </row>
@@ -9518,7 +9592,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14047,6 +14121,43 @@
         <v>112</v>
       </c>
       <c r="I122" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>45909.4343287037</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>0x00,0x70</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>130</v>
+      </c>
+      <c r="G123" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H123" t="n">
+        <v>112</v>
+      </c>
+      <c r="I123" t="n">
         <v>7</v>
       </c>
     </row>
@@ -14061,7 +14172,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18593,6 +18704,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>45909.4343287037</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>0x00,0x6E</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>130</v>
+      </c>
+      <c r="G123" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H123" t="n">
+        <v>110</v>
+      </c>
+      <c r="I123" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert data parsing logic
Update dependencies to their latest versions.
Improve performance by optimizing database queries.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5183,6 +5183,43 @@
         <v>260</v>
       </c>
       <c r="I128" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="n">
+        <v>45915.43659722222</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>0x01,0x04</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F129" t="n">
+        <v>380</v>
+      </c>
+      <c r="G129" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H129" t="n">
+        <v>260</v>
+      </c>
+      <c r="I129" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5197,7 +5234,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9948,6 +9985,43 @@
         <v>268</v>
       </c>
       <c r="I128" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="n">
+        <v>45915.43659722222</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>0x01,0x0C</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F129" t="n">
+        <v>380</v>
+      </c>
+      <c r="G129" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H129" t="n">
+        <v>268</v>
+      </c>
+      <c r="I129" t="n">
         <v>14</v>
       </c>
     </row>
@@ -9962,7 +10036,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14713,6 +14787,43 @@
         <v>111</v>
       </c>
       <c r="I128" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="n">
+        <v>45915.43659722222</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>0x00,0x6F</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F129" t="n">
+        <v>130</v>
+      </c>
+      <c r="G129" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H129" t="n">
+        <v>111</v>
+      </c>
+      <c r="I129" t="n">
         <v>7</v>
       </c>
     </row>
@@ -14727,7 +14838,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19481,6 +19592,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="129">
+      <c r="A129" s="2" t="n">
+        <v>45915.43659722222</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>0x00,0x6D</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F129" t="n">
+        <v>130</v>
+      </c>
+      <c r="G129" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H129" t="n">
+        <v>109</v>
+      </c>
+      <c r="I129" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add api response formatting
Address edge cases reported in user feedback.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5368,6 +5368,43 @@
         <v>256</v>
       </c>
       <c r="I133" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>45920.43671296296</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>0x01,0x00</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>380</v>
+      </c>
+      <c r="G134" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H134" t="n">
+        <v>256</v>
+      </c>
+      <c r="I134" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5382,7 +5419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10318,6 +10355,43 @@
         <v>264</v>
       </c>
       <c r="I133" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>45920.43671296296</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>0x01,0x04</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>380</v>
+      </c>
+      <c r="G134" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H134" t="n">
+        <v>260</v>
+      </c>
+      <c r="I134" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10332,7 +10406,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15268,6 +15342,43 @@
         <v>111</v>
       </c>
       <c r="I133" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>45920.43671296296</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>0x00,0x6F</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>130</v>
+      </c>
+      <c r="G134" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H134" t="n">
+        <v>111</v>
+      </c>
+      <c r="I134" t="n">
         <v>7</v>
       </c>
     </row>
@@ -15282,7 +15393,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20221,6 +20332,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>45920.43671296296</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>0x00,0x6C</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>130</v>
+      </c>
+      <c r="G134" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H134" t="n">
+        <v>108</v>
+      </c>
+      <c r="I134" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Optimize login page ui elements
Apply code style fixes as per linter recommendations.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:I135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5405,6 +5405,43 @@
         <v>256</v>
       </c>
       <c r="I134" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="n">
+        <v>45921.43438657407</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>0x01,0x00</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>380</v>
+      </c>
+      <c r="G135" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H135" t="n">
+        <v>256</v>
+      </c>
+      <c r="I135" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5419,7 +5456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:I135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10392,6 +10429,43 @@
         <v>260</v>
       </c>
       <c r="I134" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="n">
+        <v>45921.43438657407</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>0x01,0x04</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>380</v>
+      </c>
+      <c r="G135" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H135" t="n">
+        <v>260</v>
+      </c>
+      <c r="I135" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10406,7 +10480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:I135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15379,6 +15453,43 @@
         <v>111</v>
       </c>
       <c r="I134" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="n">
+        <v>45921.43438657407</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>0x00,0x6E</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>130</v>
+      </c>
+      <c r="G135" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H135" t="n">
+        <v>110</v>
+      </c>
+      <c r="I135" t="n">
         <v>7</v>
       </c>
     </row>
@@ -15393,7 +15504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:I135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20369,6 +20480,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="135">
+      <c r="A135" s="2" t="n">
+        <v>45921.43438657407</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>0x00,0x6C</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>130</v>
+      </c>
+      <c r="G135" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H135" t="n">
+        <v>108</v>
+      </c>
+      <c r="I135" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove file upload functionality
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5442,6 +5442,43 @@
         <v>256</v>
       </c>
       <c r="I135" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>45922.43708333333</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>0x01,0x00</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>380</v>
+      </c>
+      <c r="G136" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H136" t="n">
+        <v>256</v>
+      </c>
+      <c r="I136" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5456,7 +5493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10466,6 +10503,43 @@
         <v>260</v>
       </c>
       <c r="I135" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>45922.43708333333</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>0x01,0x04</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>380</v>
+      </c>
+      <c r="G136" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H136" t="n">
+        <v>260</v>
+      </c>
+      <c r="I136" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10480,7 +10554,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15490,6 +15564,43 @@
         <v>110</v>
       </c>
       <c r="I135" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>45922.43708333333</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>0x00,0x6E</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>130</v>
+      </c>
+      <c r="G136" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H136" t="n">
+        <v>110</v>
+      </c>
+      <c r="I136" t="n">
         <v>7</v>
       </c>
     </row>
@@ -15504,7 +15615,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20517,6 +20628,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>45922.43708333333</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>0x00,0x6C</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>130</v>
+      </c>
+      <c r="G136" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H136" t="n">
+        <v>108</v>
+      </c>
+      <c r="I136" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Simplify config file handling
Correct null value handling in data processing.
Improve performance by optimizing database queries.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I136"/>
+  <dimension ref="A1:I137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5479,6 +5479,43 @@
         <v>256</v>
       </c>
       <c r="I136" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="n">
+        <v>45923.43273148148</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>0x00,0xFC</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>380</v>
+      </c>
+      <c r="G137" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H137" t="n">
+        <v>252</v>
+      </c>
+      <c r="I137" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5493,7 +5530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I136"/>
+  <dimension ref="A1:I137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10540,6 +10577,43 @@
         <v>260</v>
       </c>
       <c r="I136" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="n">
+        <v>45923.43273148148</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>0x01,0x00</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>380</v>
+      </c>
+      <c r="G137" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H137" t="n">
+        <v>256</v>
+      </c>
+      <c r="I137" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10554,7 +10628,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I136"/>
+  <dimension ref="A1:I137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15601,6 +15675,43 @@
         <v>110</v>
       </c>
       <c r="I136" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="n">
+        <v>45923.43273148148</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>0x00,0x6E</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>130</v>
+      </c>
+      <c r="G137" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H137" t="n">
+        <v>110</v>
+      </c>
+      <c r="I137" t="n">
         <v>7</v>
       </c>
     </row>
@@ -15615,7 +15726,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I136"/>
+  <dimension ref="A1:I137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20665,6 +20776,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="137">
+      <c r="A137" s="2" t="n">
+        <v>45923.43273148148</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>0x00,0x6C</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>130</v>
+      </c>
+      <c r="G137" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H137" t="n">
+        <v>108</v>
+      </c>
+      <c r="I137" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revise csv module error handling
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I137"/>
+  <dimension ref="A1:I138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5516,6 +5516,43 @@
         <v>252</v>
       </c>
       <c r="I137" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="n">
+        <v>45924.43590277778</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>0x00,0xFC</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>380</v>
+      </c>
+      <c r="G138" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H138" t="n">
+        <v>252</v>
+      </c>
+      <c r="I138" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5530,7 +5567,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I137"/>
+  <dimension ref="A1:I138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10614,6 +10651,43 @@
         <v>256</v>
       </c>
       <c r="I137" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="n">
+        <v>45924.43590277778</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>0x01,0x00</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>380</v>
+      </c>
+      <c r="G138" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H138" t="n">
+        <v>256</v>
+      </c>
+      <c r="I138" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10628,7 +10702,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I137"/>
+  <dimension ref="A1:I138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15712,6 +15786,43 @@
         <v>110</v>
       </c>
       <c r="I137" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="n">
+        <v>45924.43590277778</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>0x00,0x6D</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>130</v>
+      </c>
+      <c r="G138" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H138" t="n">
+        <v>109</v>
+      </c>
+      <c r="I138" t="n">
         <v>7</v>
       </c>
     </row>
@@ -15726,7 +15837,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I137"/>
+  <dimension ref="A1:I138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20813,6 +20924,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="138">
+      <c r="A138" s="2" t="n">
+        <v>45924.43590277778</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>0x00,0x6C</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>130</v>
+      </c>
+      <c r="G138" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H138" t="n">
+        <v>108</v>
+      </c>
+      <c r="I138" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve logging system configuration
Optimize image compression algorithm.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I138"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5553,6 +5553,43 @@
         <v>252</v>
       </c>
       <c r="I138" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="n">
+        <v>45925.43934027778</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>0x00,0xFC</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>380</v>
+      </c>
+      <c r="G139" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H139" t="n">
+        <v>252</v>
+      </c>
+      <c r="I139" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5567,7 +5604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I138"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10688,6 +10725,43 @@
         <v>256</v>
       </c>
       <c r="I138" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="n">
+        <v>45925.43934027778</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>0x00,0xFC</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>380</v>
+      </c>
+      <c r="G139" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H139" t="n">
+        <v>252</v>
+      </c>
+      <c r="I139" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10702,7 +10776,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I138"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15823,6 +15897,43 @@
         <v>109</v>
       </c>
       <c r="I138" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="n">
+        <v>45925.43934027778</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>0x00,0x6D</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>130</v>
+      </c>
+      <c r="G139" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H139" t="n">
+        <v>109</v>
+      </c>
+      <c r="I139" t="n">
         <v>7</v>
       </c>
     </row>
@@ -15837,7 +15948,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I138"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20961,6 +21072,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="139">
+      <c r="A139" s="2" t="n">
+        <v>45925.43934027778</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>0x00,0x6C</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>130</v>
+      </c>
+      <c r="G139" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H139" t="n">
+        <v>108</v>
+      </c>
+      <c r="I139" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update user authentication module
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I140"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5627,6 +5627,43 @@
         <v>252</v>
       </c>
       <c r="I140" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="n">
+        <v>45927.43657407408</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>0x00,0xF8</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>380</v>
+      </c>
+      <c r="G141" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H141" t="n">
+        <v>248</v>
+      </c>
+      <c r="I141" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5641,7 +5678,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I140"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10836,6 +10873,43 @@
         <v>252</v>
       </c>
       <c r="I140" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="n">
+        <v>45927.43657407408</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>0x00,0xFC</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>380</v>
+      </c>
+      <c r="G141" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H141" t="n">
+        <v>252</v>
+      </c>
+      <c r="I141" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10850,7 +10924,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I140"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16045,6 +16119,43 @@
         <v>109</v>
       </c>
       <c r="I140" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="n">
+        <v>45927.43657407408</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>0x00,0x6D</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>130</v>
+      </c>
+      <c r="G141" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H141" t="n">
+        <v>109</v>
+      </c>
+      <c r="I141" t="n">
         <v>7</v>
       </c>
     </row>
@@ -16059,7 +16170,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I140"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21257,6 +21368,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="141">
+      <c r="A141" s="2" t="n">
+        <v>45927.43657407408</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>0x00,0x6B</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>130</v>
+      </c>
+      <c r="G141" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H141" t="n">
+        <v>107</v>
+      </c>
+      <c r="I141" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Simplify api response formatting
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I141"/>
+  <dimension ref="A1:I142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5664,6 +5664,43 @@
         <v>248</v>
       </c>
       <c r="I141" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="n">
+        <v>45928.43809027778</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>0x00,0xF8</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>380</v>
+      </c>
+      <c r="G142" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H142" t="n">
+        <v>248</v>
+      </c>
+      <c r="I142" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5678,7 +5715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I141"/>
+  <dimension ref="A1:I142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10910,6 +10947,43 @@
         <v>252</v>
       </c>
       <c r="I141" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="n">
+        <v>45928.43809027778</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>0x00,0xFC</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>380</v>
+      </c>
+      <c r="G142" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H142" t="n">
+        <v>252</v>
+      </c>
+      <c r="I142" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10924,7 +10998,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I141"/>
+  <dimension ref="A1:I142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16156,6 +16230,43 @@
         <v>109</v>
       </c>
       <c r="I141" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="n">
+        <v>45928.43809027778</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>0x00,0x6D</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>130</v>
+      </c>
+      <c r="G142" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H142" t="n">
+        <v>109</v>
+      </c>
+      <c r="I142" t="n">
         <v>7</v>
       </c>
     </row>
@@ -16170,7 +16281,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I141"/>
+  <dimension ref="A1:I142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21405,6 +21516,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="142">
+      <c r="A142" s="2" t="n">
+        <v>45928.43809027778</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>0x00,0x6B</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>130</v>
+      </c>
+      <c r="G142" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H142" t="n">
+        <v>107</v>
+      </c>
+      <c r="I142" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upgrade file upload functionality
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I148"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5923,6 +5923,43 @@
         <v>240</v>
       </c>
       <c r="I148" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>45935.43868055556</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>0x00,0xF0</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>380</v>
+      </c>
+      <c r="G149" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H149" t="n">
+        <v>240</v>
+      </c>
+      <c r="I149" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5937,7 +5974,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I148"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11428,6 +11465,43 @@
         <v>248</v>
       </c>
       <c r="I148" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>45935.43868055556</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>0x00,0xF4</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>380</v>
+      </c>
+      <c r="G149" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H149" t="n">
+        <v>244</v>
+      </c>
+      <c r="I149" t="n">
         <v>14</v>
       </c>
     </row>
@@ -11442,7 +11516,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I148"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16933,6 +17007,43 @@
         <v>108</v>
       </c>
       <c r="I148" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>45935.43868055556</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>0x00,0x6C</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>130</v>
+      </c>
+      <c r="G149" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H149" t="n">
+        <v>108</v>
+      </c>
+      <c r="I149" t="n">
         <v>7</v>
       </c>
     </row>
@@ -16947,7 +17058,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I148"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22441,6 +22552,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>45935.43868055556</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>0x00,0x69</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>130</v>
+      </c>
+      <c r="G149" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H149" t="n">
+        <v>105</v>
+      </c>
+      <c r="I149" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove data parsing logic
Fix various typos in comments and documentation.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I149"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5960,6 +5960,43 @@
         <v>240</v>
       </c>
       <c r="I149" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>45936.43359953703</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>0x00,0xEC</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>380</v>
+      </c>
+      <c r="G150" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H150" t="n">
+        <v>236</v>
+      </c>
+      <c r="I150" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5974,7 +6011,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I149"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11502,6 +11539,43 @@
         <v>244</v>
       </c>
       <c r="I149" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>45936.43359953703</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>0x00,0xF4</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>380</v>
+      </c>
+      <c r="G150" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H150" t="n">
+        <v>244</v>
+      </c>
+      <c r="I150" t="n">
         <v>14</v>
       </c>
     </row>
@@ -11516,7 +11590,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I149"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17044,6 +17118,43 @@
         <v>108</v>
       </c>
       <c r="I149" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>45936.43359953703</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>0x00,0x6B</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>130</v>
+      </c>
+      <c r="G150" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H150" t="n">
+        <v>107</v>
+      </c>
+      <c r="I150" t="n">
         <v>7</v>
       </c>
     </row>
@@ -17058,7 +17169,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I149"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22589,6 +22700,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>45936.43359953703</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>0x00,0x69</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>130</v>
+      </c>
+      <c r="G150" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H150" t="n">
+        <v>105</v>
+      </c>
+      <c r="I150" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Correct api response formatting
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I151"/>
+  <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6034,6 +6034,43 @@
         <v>236</v>
       </c>
       <c r="I151" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="n">
+        <v>45938.43517361111</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>0x00,0xEC</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>380</v>
+      </c>
+      <c r="G152" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H152" t="n">
+        <v>236</v>
+      </c>
+      <c r="I152" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6048,7 +6085,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I151"/>
+  <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11650,6 +11687,43 @@
         <v>244</v>
       </c>
       <c r="I151" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="n">
+        <v>45938.43517361111</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>0x00,0xF4</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>380</v>
+      </c>
+      <c r="G152" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H152" t="n">
+        <v>244</v>
+      </c>
+      <c r="I152" t="n">
         <v>14</v>
       </c>
     </row>
@@ -11664,7 +11738,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I151"/>
+  <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17266,6 +17340,43 @@
         <v>107</v>
       </c>
       <c r="I151" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="n">
+        <v>45938.43517361111</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>0x00,0x6B</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>130</v>
+      </c>
+      <c r="G152" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H152" t="n">
+        <v>107</v>
+      </c>
+      <c r="I152" t="n">
         <v>7</v>
       </c>
     </row>
@@ -17280,7 +17391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I151"/>
+  <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22885,6 +22996,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="152">
+      <c r="A152" s="2" t="n">
+        <v>45938.43517361111</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>0x00,0x69</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>130</v>
+      </c>
+      <c r="G152" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H152" t="n">
+        <v>105</v>
+      </c>
+      <c r="I152" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update database schema migration
Simplify code structure to improve readability.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6256,6 +6256,43 @@
         <v>232</v>
       </c>
       <c r="I157" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>45944.43943287037</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>0x00,0xE8</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>380</v>
+      </c>
+      <c r="G158" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H158" t="n">
+        <v>232</v>
+      </c>
+      <c r="I158" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6270,7 +6307,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12094,6 +12131,43 @@
         <v>240</v>
       </c>
       <c r="I157" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>45944.43943287037</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>0x00,0xEC</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>380</v>
+      </c>
+      <c r="G158" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H158" t="n">
+        <v>236</v>
+      </c>
+      <c r="I158" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12108,7 +12182,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17932,6 +18006,43 @@
         <v>107</v>
       </c>
       <c r="I157" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>45944.43943287037</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>0x00,0x6A</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>130</v>
+      </c>
+      <c r="G158" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H158" t="n">
+        <v>106</v>
+      </c>
+      <c r="I158" t="n">
         <v>7</v>
       </c>
     </row>
@@ -17946,7 +18057,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23773,6 +23884,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>45944.43943287037</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>0x00,0x68</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>130</v>
+      </c>
+      <c r="G158" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H158" t="n">
+        <v>104</v>
+      </c>
+      <c r="I158" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert build script optimization
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I160"/>
+  <dimension ref="A1:I161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6367,6 +6367,43 @@
         <v>228</v>
       </c>
       <c r="I160" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>45947.43653935185</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>0x00,0xE4</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F161" t="n">
+        <v>380</v>
+      </c>
+      <c r="G161" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H161" t="n">
+        <v>228</v>
+      </c>
+      <c r="I161" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6381,7 +6418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I160"/>
+  <dimension ref="A1:I161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12316,6 +12353,43 @@
         <v>236</v>
       </c>
       <c r="I160" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>45947.43653935185</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>0x00,0xEC</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F161" t="n">
+        <v>380</v>
+      </c>
+      <c r="G161" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H161" t="n">
+        <v>236</v>
+      </c>
+      <c r="I161" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12330,7 +12404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I160"/>
+  <dimension ref="A1:I161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18265,6 +18339,43 @@
         <v>106</v>
       </c>
       <c r="I160" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>45947.43653935185</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>0x00,0x6A</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F161" t="n">
+        <v>130</v>
+      </c>
+      <c r="G161" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H161" t="n">
+        <v>106</v>
+      </c>
+      <c r="I161" t="n">
         <v>7</v>
       </c>
     </row>
@@ -18279,7 +18390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I160"/>
+  <dimension ref="A1:I161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24217,6 +24328,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>45947.43653935185</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>0x00,0x67</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F161" t="n">
+        <v>130</v>
+      </c>
+      <c r="G161" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H161" t="n">
+        <v>103</v>
+      </c>
+      <c r="I161" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add navigation menu accessibility
Add input validation for better security.
Optimize image compression algorithm.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I162"/>
+  <dimension ref="A1:I163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6441,6 +6441,43 @@
         <v>228</v>
       </c>
       <c r="I162" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="n">
+        <v>45949.43864583333</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>0x00,0xE0</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F163" t="n">
+        <v>380</v>
+      </c>
+      <c r="G163" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H163" t="n">
+        <v>224</v>
+      </c>
+      <c r="I163" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6455,7 +6492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I162"/>
+  <dimension ref="A1:I163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12464,6 +12501,43 @@
         <v>236</v>
       </c>
       <c r="I162" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="n">
+        <v>45949.43864583333</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>0x00,0xE8</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F163" t="n">
+        <v>380</v>
+      </c>
+      <c r="G163" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H163" t="n">
+        <v>232</v>
+      </c>
+      <c r="I163" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12478,7 +12552,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I162"/>
+  <dimension ref="A1:I163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18487,6 +18561,43 @@
         <v>106</v>
       </c>
       <c r="I162" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="n">
+        <v>45949.43864583333</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>0x00,0x6A</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F163" t="n">
+        <v>130</v>
+      </c>
+      <c r="G163" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H163" t="n">
+        <v>106</v>
+      </c>
+      <c r="I163" t="n">
         <v>7</v>
       </c>
     </row>
@@ -18501,7 +18612,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I162"/>
+  <dimension ref="A1:I163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24513,6 +24624,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="163">
+      <c r="A163" s="2" t="n">
+        <v>45949.43864583333</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>0x00,0x67</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F163" t="n">
+        <v>130</v>
+      </c>
+      <c r="G163" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H163" t="n">
+        <v>103</v>
+      </c>
+      <c r="I163" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upgrade database schema migration
Add missing documentation for the new API.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6589,6 +6589,43 @@
         <v>220</v>
       </c>
       <c r="I166" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45953.43768518518</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>0x00,0xDC</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>380</v>
+      </c>
+      <c r="G167" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H167" t="n">
+        <v>220</v>
+      </c>
+      <c r="I167" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6603,7 +6640,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12760,6 +12797,43 @@
         <v>228</v>
       </c>
       <c r="I166" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45953.43768518518</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>0x00,0xE0</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>380</v>
+      </c>
+      <c r="G167" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H167" t="n">
+        <v>224</v>
+      </c>
+      <c r="I167" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12774,7 +12848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18931,6 +19005,43 @@
         <v>105</v>
       </c>
       <c r="I166" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45953.43768518518</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>0x00,0x69</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>130</v>
+      </c>
+      <c r="G167" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H167" t="n">
+        <v>105</v>
+      </c>
+      <c r="I167" t="n">
         <v>7</v>
       </c>
     </row>
@@ -18945,7 +19056,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25105,6 +25216,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45953.43768518518</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>0x00,0x67</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>130</v>
+      </c>
+      <c r="G167" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H167" t="n">
+        <v>103</v>
+      </c>
+      <c r="I167" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert user authentication module
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I175"/>
+  <dimension ref="A1:I176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6922,6 +6922,43 @@
         <v>212</v>
       </c>
       <c r="I175" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="n">
+        <v>45962.43868055556</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>0x00,0xD4</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F176" t="n">
+        <v>380</v>
+      </c>
+      <c r="G176" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H176" t="n">
+        <v>212</v>
+      </c>
+      <c r="I176" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6936,7 +6973,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I175"/>
+  <dimension ref="A1:I176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13426,6 +13463,43 @@
         <v>220</v>
       </c>
       <c r="I175" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="n">
+        <v>45962.43868055556</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>0x00,0xDC</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F176" t="n">
+        <v>380</v>
+      </c>
+      <c r="G176" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H176" t="n">
+        <v>220</v>
+      </c>
+      <c r="I176" t="n">
         <v>14</v>
       </c>
     </row>
@@ -13440,7 +13514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I175"/>
+  <dimension ref="A1:I176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19930,6 +20004,43 @@
         <v>103</v>
       </c>
       <c r="I175" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="n">
+        <v>45962.43868055556</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>0x00,0x67</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F176" t="n">
+        <v>130</v>
+      </c>
+      <c r="G176" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H176" t="n">
+        <v>103</v>
+      </c>
+      <c r="I176" t="n">
         <v>7</v>
       </c>
     </row>
@@ -19944,7 +20055,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I175"/>
+  <dimension ref="A1:I176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26437,6 +26548,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="176">
+      <c r="A176" s="2" t="n">
+        <v>45962.43868055556</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>0x00,0x64</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F176" t="n">
+        <v>130</v>
+      </c>
+      <c r="G176" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H176" t="n">
+        <v>100</v>
+      </c>
+      <c r="I176" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>